<commit_message>
Added project progress tracker.
Created basic tracker to kep note of progress and plan next steps.
</commit_message>
<xml_diff>
--- a/documentation/ProjectProgress.xlsx
+++ b/documentation/ProjectProgress.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -25,13 +25,31 @@
   </si>
   <si>
     <t>Got Arduino and STK600 with UC3C0512C to pass SPI data between one another. Arduino is master. UC3C doesn't seem to like SS line toggling between data transfers. Need to investigate this further. Check UC3C datasheet for SPI timings. Could simply be that the oscillator and clock tree is not yet set up.</t>
+  </si>
+  <si>
+    <t>FIxed SPI Slave Select issue. Need to insert a small delay between end of SPI transfer and rising edge of SS signal. Without the delay, SS rises 4.5us after end of transfer. This would seem to be in spec according to datasheet, but may be affected due to not having set up UC3C oscillator and clock tree correctly.</t>
+  </si>
+  <si>
+    <t>See Also</t>
+  </si>
+  <si>
+    <t>SPI-transfer-1.png</t>
+  </si>
+  <si>
+    <t>SPI-transfer-2.png</t>
+  </si>
+  <si>
+    <t>SPI-transfer-3-SS-Rises-Too-Early.png</t>
+  </si>
+  <si>
+    <t>SPI-transfer-4-SS-Rises-Too-Early.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -46,6 +64,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -62,7 +87,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -70,11 +95,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right style="thick">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -82,17 +131,27 @@
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -385,35 +444,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="155.28515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="155.28515625" style="3" customWidth="1"/>
+    <col min="3" max="4" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="35.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="37.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:2" ht="30">
-      <c r="A2" s="5">
+    <row r="2" spans="1:9" ht="30">
+      <c r="A2" s="4">
         <v>41118</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30">
+      <c r="A3" s="4">
+        <v>41118</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:I1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId3"/>
+    <hyperlink ref="F3" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added TODO list to Excel file.
</commit_message>
<xml_diff>
--- a/documentation/ProjectProgress.xlsx
+++ b/documentation/ProjectProgress.xlsx
@@ -4,15 +4,17 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="6645" windowHeight="8565"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="6645" windowHeight="8565" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ProgressTracker" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="5-Byte-Transfer" sheetId="3" r:id="rId3"/>
+    <sheet name="TODO" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="5-Byte-Transfer" sheetId="3" r:id="rId4"/>
+    <sheet name="MissingModels" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="full_speed_5_byte_transfer" localSheetId="2">'5-Byte-Transfer'!$A$1:$E$1244</definedName>
+    <definedName name="full_speed_5_byte_transfer" localSheetId="3">'5-Byte-Transfer'!$A$1:$E$1244</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="1264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="1279">
   <si>
     <t>Date</t>
   </si>
@@ -3827,6 +3829,51 @@
   </si>
   <si>
     <t>Decided to rip-up LC board and start again. Using surface mount headers to connect to Arduino as there is simply no space for the QTouch sensor headers otherwise. Now header for Arduino are on bottom, and QTouch headers on top.</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>TASK</t>
+  </si>
+  <si>
+    <t>Check that the RX/TX pins of UC3C go to the TX/RX (i.e. they are correctly swapped) of the Arduino platform</t>
+  </si>
+  <si>
+    <t>Build a QTouch example using the library and the STK600 - ensure STK600 can be debugged using QT600 interface board and QTouch Studio</t>
+  </si>
+  <si>
+    <t>Check the USB interface requirements for USB-Host on UC3C. Specifically, how is the Pin 1 Vcc connected to the UC3C? Directly, or via a switch (transistor) circuit?</t>
+  </si>
+  <si>
+    <t>Check orientation of JTAG header - where is pin 1?</t>
+  </si>
+  <si>
+    <t>Check orientation of QT600 debug date header - where is pin 1?</t>
+  </si>
+  <si>
+    <t>2X8-V-MALE-SMT-HARWIN</t>
+  </si>
+  <si>
+    <t>2X8-V-FEMALE-SMT-HARWIN</t>
+  </si>
+  <si>
+    <t>2X4-V-MALE-SMT-HARWIN</t>
+  </si>
+  <si>
+    <t>LED-1206</t>
+  </si>
+  <si>
+    <t>SOT23-3</t>
+  </si>
+  <si>
+    <t>SJ</t>
+  </si>
+  <si>
+    <t>ARDUINO-2560-R3-SMD</t>
+  </si>
+  <si>
+    <t>PN87520</t>
   </si>
 </sst>
 </file>
@@ -3907,7 +3954,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3940,6 +3987,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -18939,24 +18995,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="102615680"/>
-        <c:axId val="102236544"/>
+        <c:axId val="113029888"/>
+        <c:axId val="114667520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102615680"/>
+        <c:axId val="113029888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102236544"/>
+        <c:crossAx val="114667520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102236544"/>
+        <c:axId val="114667520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18964,19 +19020,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102615680"/>
+        <c:crossAx val="113029888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -19308,8 +19365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19430,6 +19487,136 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="118.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="47.25" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="12" customFormat="1">
+      <c r="A2" s="12" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="12" customFormat="1" ht="30">
+      <c r="A3" s="12" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30">
+      <c r="A4" s="13" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="13" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="13" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="13"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="13"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="13"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="13"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="13"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="13"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="13"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="13"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="13"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="13"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="13"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="13"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="13"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="13"/>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="13"/>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="13"/>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="13"/>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="13"/>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="13"/>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="13"/>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="13"/>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="13"/>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="13"/>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="13"/>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="13"/>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19580,7 +19767,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J1244"/>
   <sheetViews>
@@ -60648,4 +60835,72 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="14">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="14">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="14" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="14" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="14" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="14" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="14" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="14" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="14" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="14" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update progress on board.
</commit_message>
<xml_diff>
--- a/documentation/ProjectProgress.xlsx
+++ b/documentation/ProjectProgress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="6645" windowHeight="8565" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="6645" windowHeight="8565" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ProgressTracker" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="1279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="1281">
   <si>
     <t>Date</t>
   </si>
@@ -3874,6 +3874,12 @@
   </si>
   <si>
     <t>PN87520</t>
+  </si>
+  <si>
+    <t>Added 10uF cap on VCC after review with STROHAL</t>
+  </si>
+  <si>
+    <t>Around 95% routed. Added in-line resistors in D+/D- USB lines. NOTE: RESET from JTAG goes to UC3 RESET; RESET from Arduino board goes to cuttable jumper.</t>
   </si>
 </sst>
 </file>
@@ -3981,12 +3987,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3995,6 +3995,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -18995,24 +19001,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="113029888"/>
-        <c:axId val="114667520"/>
+        <c:axId val="109889024"/>
+        <c:axId val="109890560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="113029888"/>
+        <c:axId val="109889024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114667520"/>
+        <c:crossAx val="109890560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114667520"/>
+        <c:axId val="109890560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19020,20 +19026,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113029888"/>
+        <c:crossAx val="109889024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -19363,10 +19368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19385,15 +19390,15 @@
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:9" ht="30">
       <c r="A2" s="4">
@@ -19467,6 +19472,22 @@
       </c>
       <c r="B8" s="3" t="s">
         <v>1263</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="4">
+        <v>41129</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="4">
+        <v>41130</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>1280</v>
       </c>
     </row>
   </sheetData>
@@ -19489,7 +19510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -19507,108 +19528,108 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="12" customFormat="1">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:2" s="10" customFormat="1">
+      <c r="A2" s="10" t="s">
         <v>1266</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="12" customFormat="1" ht="30">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:2" s="10" customFormat="1" ht="30">
+      <c r="A3" s="10" t="s">
         <v>1267</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>1268</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>1269</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>1270</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="13"/>
+      <c r="A7" s="11"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="13"/>
+      <c r="A8" s="11"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="13"/>
+      <c r="A9" s="11"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="13"/>
+      <c r="A10" s="11"/>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="13"/>
+      <c r="A11" s="11"/>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="13"/>
+      <c r="A12" s="11"/>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="13"/>
+      <c r="A13" s="11"/>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="13"/>
+      <c r="A14" s="11"/>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="13"/>
+      <c r="A15" s="11"/>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="13"/>
+      <c r="A16" s="11"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="13"/>
+      <c r="A17" s="11"/>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="13"/>
+      <c r="A18" s="11"/>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="13"/>
+      <c r="A19" s="11"/>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="13"/>
+      <c r="A20" s="11"/>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="13"/>
+      <c r="A21" s="11"/>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="13"/>
+      <c r="A22" s="11"/>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="13"/>
+      <c r="A23" s="11"/>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="13"/>
+      <c r="A24" s="11"/>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="13"/>
+      <c r="A25" s="11"/>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="13"/>
+      <c r="A26" s="11"/>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="13"/>
+      <c r="A27" s="11"/>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="13"/>
+      <c r="A28" s="11"/>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="13"/>
+      <c r="A29" s="11"/>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="13"/>
+      <c r="A30" s="11"/>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="13"/>
+      <c r="A31" s="11"/>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="13"/>
+      <c r="A32" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -60841,7 +60862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -60851,52 +60872,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="14">
+      <c r="A1" s="12">
         <v>805</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="14">
+      <c r="A2" s="12">
         <v>1210</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="12" t="s">
         <v>1271</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="12" t="s">
         <v>1272</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="12" t="s">
         <v>1273</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="12" t="s">
         <v>1274</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="12" t="s">
         <v>1275</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="12" t="s">
         <v>1276</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="12" t="s">
         <v>1277</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="12" t="s">
         <v>1278</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update of project progess and todo: list
</commit_message>
<xml_diff>
--- a/documentation/ProjectProgress.xlsx
+++ b/documentation/ProjectProgress.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="1281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="1282">
   <si>
     <t>Date</t>
   </si>
@@ -3880,6 +3880,9 @@
   </si>
   <si>
     <t>Around 95% routed. Added in-line resistors in D+/D- USB lines. NOTE: RESET from JTAG goes to UC3 RESET; RESET from Arduino board goes to cuttable jumper.</t>
+  </si>
+  <si>
+    <t>Check availability of parts in specified package sizes.</t>
   </si>
 </sst>
 </file>
@@ -19001,24 +19004,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="109889024"/>
-        <c:axId val="109890560"/>
+        <c:axId val="99227904"/>
+        <c:axId val="101372672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109889024"/>
+        <c:axId val="99227904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109890560"/>
+        <c:crossAx val="101372672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109890560"/>
+        <c:axId val="101372672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19026,7 +19029,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109889024"/>
+        <c:crossAx val="99227904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19038,7 +19041,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -19511,7 +19514,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19554,7 +19557,9 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="11"/>
+      <c r="A7" s="11" t="s">
+        <v>1281</v>
+      </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="11"/>

</xml_diff>